<commit_message>
Add data loader module
</commit_message>
<xml_diff>
--- a/positions_example.xlsx
+++ b/positions_example.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Company</t>
+          <t>公司名字</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Position</t>
+          <t>岗位名</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>地点</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Job_Description</t>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>job description</t>
         </is>
       </c>
     </row>
@@ -473,6 +478,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>https://techcorp.com/careers/swe-intern</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>We are seeking a Software Engineer Intern to join our backend development team. The intern will work on designing and implementing scalable web services using Java and Spring Boot. Responsibilities include developing RESTful APIs, working with databases, and collaborating with senior engineers on system architecture. No citizenship requirements. This is an entry-level internship position perfect for students.</t>
         </is>
       </c>
@@ -495,6 +505,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>https://aisolutions.com/jobs/mle-intern</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Looking for a Machine Learning Engineer Intern to help build and deploy AI models in production. The role involves working with Python, TensorFlow, and AWS to create recommendation systems and computer vision applications. The intern will collaborate with data scientists and software engineers to optimize model performance. This internship is open to all students regardless of citizenship status. No prior industry experience required.</t>
         </is>
       </c>
@@ -516,6 +531,11 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>https://dataflow.com/careers/quant-intern</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Quantitative Research Intern position available for students interested in algorithmic trading and financial modeling. The role requires strong mathematical background and programming skills in Python or R. Intern will develop trading strategies, perform statistical analysis, and work with large financial datasets. This position requires US citizenship or permanent residency due to regulatory compliance requirements.</t>
         </is>

</xml_diff>

<commit_message>
Update data loader: add multi-sheet and date range filtering support
</commit_message>
<xml_diff>
--- a/positions_example.xlsx
+++ b/positions_example.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>日期</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>job description</t>
         </is>
       </c>
@@ -483,6 +488,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>We are seeking a Software Engineer Intern to join our backend development team. The intern will work on designing and implementing scalable web services using Java and Spring Boot. Responsibilities include developing RESTful APIs, working with databases, and collaborating with senior engineers on system architecture. No citizenship requirements. This is an entry-level internship position perfect for students.</t>
         </is>
       </c>
@@ -510,6 +520,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>2024-01-20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Looking for a Machine Learning Engineer Intern to help build and deploy AI models in production. The role involves working with Python, TensorFlow, and AWS to create recommendation systems and computer vision applications. The intern will collaborate with data scientists and software engineers to optimize model performance. This internship is open to all students regardless of citizenship status. No prior industry experience required.</t>
         </is>
       </c>
@@ -536,6 +551,11 @@
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-01-25</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Quantitative Research Intern position available for students interested in algorithmic trading and financial modeling. The role requires strong mathematical background and programming skills in Python or R. Intern will develop trading strategies, perform statistical analysis, and work with large financial datasets. This position requires US citizenship or permanent residency due to regulatory compliance requirements.</t>
         </is>

</xml_diff>

<commit_message>
Refactor: Split LLM clients into modular architecture
- Split llm_clients.py into modular components
- Created utils/ for JSONFixer
- Created config/ for PromptManager
- Created llm/ with base_client and individual clients
- Improved code organization and maintainability
- Added unified LLM manager with async/concurrent support
</commit_message>
<xml_diff>
--- a/positions_example.xlsx
+++ b/positions_example.xlsx
@@ -1,37 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangziye/Desktop/CV/code/resume-optimizer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637F95F-C037-CE4F-804F-1CAD0A918FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>公司名字</t>
+  </si>
+  <si>
+    <t>岗位名</t>
+  </si>
+  <si>
+    <t>地点</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>日期</t>
+  </si>
+  <si>
+    <t>job description</t>
+  </si>
+  <si>
+    <t>TechCorp Inc.</t>
+  </si>
+  <si>
+    <t>Software Engineer Intern</t>
+  </si>
+  <si>
+    <t>San Francisco, CA</t>
+  </si>
+  <si>
+    <t>https://techcorp.com/careers/swe-intern</t>
+  </si>
+  <si>
+    <t>2024-01-15</t>
+  </si>
+  <si>
+    <t>We are seeking a Software Engineer Intern to join our backend development team. The intern will work on designing and implementing scalable web services using Java and Spring Boot. Responsibilities include developing RESTful APIs, working with databases, and collaborating with senior engineers on system architecture. No citizenship requirements. This is an entry-level internship position perfect for students.</t>
+  </si>
+  <si>
+    <t>AI Solutions Ltd.</t>
+  </si>
+  <si>
+    <t>Machine Learning Engineer Intern</t>
+  </si>
+  <si>
+    <t>Seattle, WA</t>
+  </si>
+  <si>
+    <t>https://aisolutions.com/jobs/mle-intern</t>
+  </si>
+  <si>
+    <t>2024-01-20</t>
+  </si>
+  <si>
+    <t>Looking for a Machine Learning Engineer Intern to help build and deploy AI models in production. The role involves working with Python, TensorFlow, and AWS to create recommendation systems and computer vision applications. The intern will collaborate with data scientists and software engineers to optimize model performance. This internship is open to all students regardless of citizenship status. No prior industry experience required.</t>
+  </si>
+  <si>
+    <t>DataFlow Systems</t>
+  </si>
+  <si>
+    <t>Quantitative Research Intern</t>
+  </si>
+  <si>
+    <t>New York, NY</t>
+  </si>
+  <si>
+    <t>https://dataflow.com/careers/quant-intern</t>
+  </si>
+  <si>
+    <t>2024-01-25</t>
+  </si>
+  <si>
+    <t>Quantitative Research Intern position available for students interested in algorithmic trading and financial modeling. The role requires strong mathematical background and programming skills in Python or R. Intern will develop trading strategies, perform statistical analysis, and work with large financial datasets. This position requires US citizenship or permanent residency due to regulatory compliance requirements.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +130,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,145 +454,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>公司名字</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>岗位名</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>地点</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>link</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>日期</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>job description</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TechCorp Inc.</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Software Engineer Intern</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>San Francisco, CA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://techcorp.com/careers/swe-intern</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-01-15</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>We are seeking a Software Engineer Intern to join our backend development team. The intern will work on designing and implementing scalable web services using Java and Spring Boot. Responsibilities include developing RESTful APIs, working with databases, and collaborating with senior engineers on system architecture. No citizenship requirements. This is an entry-level internship position perfect for students.</t>
-        </is>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>AI Solutions Ltd.</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Machine Learning Engineer Intern</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Seattle, WA</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://aisolutions.com/jobs/mle-intern</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-01-20</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Looking for a Machine Learning Engineer Intern to help build and deploy AI models in production. The role involves working with Python, TensorFlow, and AWS to create recommendation systems and computer vision applications. The intern will collaborate with data scientists and software engineers to optimize model performance. This internship is open to all students regardless of citizenship status. No prior industry experience required.</t>
-        </is>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DataFlow Systems</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Quantitative Research Intern</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>New York, NY</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://dataflow.com/careers/quant-intern</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-01-25</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Quantitative Research Intern position available for students interested in algorithmic trading and financial modeling. The role requires strong mathematical background and programming skills in Python or R. Intern will develop trading strategies, perform statistical analysis, and work with large financial datasets. This position requires US citizenship or permanent residency due to regulatory compliance requirements.</t>
-        </is>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bugs for GPT and Claude
</commit_message>
<xml_diff>
--- a/positions_example.xlsx
+++ b/positions_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangziye/Desktop/CV/code/resume-optimizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637F95F-C037-CE4F-804F-1CAD0A918FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988574E5-98C4-DA42-9393-7864E90D637B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>公司名字</t>
   </si>
@@ -40,65 +40,58 @@
     <t>job description</t>
   </si>
   <si>
-    <t>TechCorp Inc.</t>
-  </si>
-  <si>
-    <t>Software Engineer Intern</t>
-  </si>
-  <si>
-    <t>San Francisco, CA</t>
-  </si>
-  <si>
-    <t>https://techcorp.com/careers/swe-intern</t>
-  </si>
-  <si>
-    <t>2024-01-15</t>
-  </si>
-  <si>
-    <t>We are seeking a Software Engineer Intern to join our backend development team. The intern will work on designing and implementing scalable web services using Java and Spring Boot. Responsibilities include developing RESTful APIs, working with databases, and collaborating with senior engineers on system architecture. No citizenship requirements. This is an entry-level internship position perfect for students.</t>
-  </si>
-  <si>
-    <t>AI Solutions Ltd.</t>
-  </si>
-  <si>
-    <t>Machine Learning Engineer Intern</t>
-  </si>
-  <si>
-    <t>Seattle, WA</t>
-  </si>
-  <si>
-    <t>https://aisolutions.com/jobs/mle-intern</t>
-  </si>
-  <si>
-    <t>2024-01-20</t>
-  </si>
-  <si>
-    <t>Looking for a Machine Learning Engineer Intern to help build and deploy AI models in production. The role involves working with Python, TensorFlow, and AWS to create recommendation systems and computer vision applications. The intern will collaborate with data scientists and software engineers to optimize model performance. This internship is open to all students regardless of citizenship status. No prior industry experience required.</t>
-  </si>
-  <si>
-    <t>DataFlow Systems</t>
-  </si>
-  <si>
-    <t>Quantitative Research Intern</t>
-  </si>
-  <si>
-    <t>New York, NY</t>
-  </si>
-  <si>
-    <t>https://dataflow.com/careers/quant-intern</t>
-  </si>
-  <si>
-    <t>2024-01-25</t>
-  </si>
-  <si>
-    <t>Quantitative Research Intern position available for students interested in algorithmic trading and financial modeling. The role requires strong mathematical background and programming skills in Python or R. Intern will develop trading strategies, perform statistical analysis, and work with large financial datasets. This position requires US citizenship or permanent residency due to regulatory compliance requirements.</t>
+    <t>Sigiq</t>
+  </si>
+  <si>
+    <t>Berkeley, CA</t>
+  </si>
+  <si>
+    <t>Machine learning engineer</t>
+  </si>
+  <si>
+    <t>https://app.dover.com/apply/SigIQ.ai/9d3a9bb3-aa1e-48dd-8537-268ef2adaace</t>
+  </si>
+  <si>
+    <t>🚀 About SigIQ.ai
+SigIQ.ai is building the operating system for AI-native education. Our tutors combine LLMs with real student data to deliver feedback in seconds, not semesters.
+What we’ve built so far:
+PadhAI served 200K+ learners and outperformed GPT-4o on a national exam
+EverTutor hit 10K users in 90 days and improved GRE outcomes by 18%
+Backed by GSV Ventures, The House Fund, Peak XV, Duolingo, and more ($9.8M seed)
+Now building ET Live, a real-time AI tutor. You’ll help bring it to life.
+You will work side by side with Dr. Karttikeya Mangalam, UC Berkeley‑trained AI researcher and founder, and Professor Kurt Keutzer, Berkeley EECS legend and serial entrepreneur.
+🎯 Role Overview
+This is an ongoing part-time internship for students who want to build real AI products alongside top researchers and engineers. You’ll join us on-site in Berkeley 2–3 days a week (we’re flexible with school schedules) and ship meaningful work, not side projects.
+🧠 What You’ll Do
+Contribute to LLM-powered tutoring systems
+Build and improve evaluation and feedback pipelines
+Prototype ML features in production-like environments
+Collaborate with product, design, and engineering
+Learn from some of the best minds in AI and education
+✅ You Might Be a Fit If You...
+Pursuing a Bachelor's or Master's degree in CS, EECS, Data Science, or a similar field
+Have strong Python skills (through classes, personal projects, or research)
+Are curious about LLMs, personalization, and real-time tutoring workflows
+Can commit to 20–25 hours/week on-site in Berkeley during the academic year
+Want mentorship, fast learning loops, and a shot at a return offer
+🚀 Bonus Points
+Experience with ML/AI frameworks (e.g., Huggingface, Pytorch, vLLM)
+Familiarity with API design, LangChain, or prompt engineering
+Past hackathon wins, GitHub repos, or ML side projects
+Interested in education, learning science, or product thinking
+🎁 What You’ll Get
+Paid internship
+Access to founders, advisors, and investors in edtech + AI
+Ownership and visibility from day one
+Return offer pathway based on performance
+A front-row seat to building AI tutors that actually teach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +104,36 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212529"/>
+      <name val="Inter"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF212529"/>
+      <name val="Inter"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,16 +168,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,15 +489,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -483,65 +517,121 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" ht="409.6">
+      <c r="A2" s="2">
+        <v>45891</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="21">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="21">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="21">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="20">
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="20">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="20">
+      <c r="F13" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="21">
+      <c r="F15" s="6"/>
+    </row>
+    <row r="17" spans="6:6" ht="20">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="19" spans="6:6" ht="21">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="21" spans="6:6" ht="20">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="6:6" ht="20">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="6:6" ht="20">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="6:6" ht="20">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="6:6" ht="20">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="27" spans="6:6" ht="21">
+      <c r="F27" s="6"/>
+    </row>
+    <row r="29" spans="6:6" ht="20">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="6:6" ht="20">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="6:6" ht="20">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="6:6" ht="20">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="6:6" ht="20">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="35" spans="6:6" ht="21">
+      <c r="F35" s="6"/>
+    </row>
+    <row r="37" spans="6:6" ht="20">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="6:6" ht="20">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="6:6" ht="20">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="6:6" ht="20">
+      <c r="F40" s="7"/>
+    </row>
+    <row r="42" spans="6:6" ht="21">
+      <c r="F42" s="6"/>
+    </row>
+    <row r="44" spans="6:6" ht="20">
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="6:6" ht="20">
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="6:6" ht="20">
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="6:6" ht="20">
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="6:6" ht="20">
+      <c r="F48" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>